<commit_message>
Excel handler refact (dynamic now)
</commit_message>
<xml_diff>
--- a/FilteredBikesData.xlsx
+++ b/FilteredBikesData.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Bikes" r:id="rId3" sheetId="1"/>
+    <sheet name="data" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -17,7 +17,7 @@
     <t>Bike Name</t>
   </si>
   <si>
-    <t>Price</t>
+    <t>Bike price</t>
   </si>
   <si>
     <t>Expected Launch Date</t>
@@ -26,7 +26,7 @@
     <t>Honda CB350 Cruiser</t>
   </si>
   <si>
-    <t>Rs. 229999</t>
+    <t>229999</t>
   </si>
   <si>
     <t>Expected Launch : Jul 2025</t>
@@ -35,7 +35,7 @@
     <t>Honda Activa 7G</t>
   </si>
   <si>
-    <t>Rs. 79000</t>
+    <t>79000</t>
   </si>
   <si>
     <t>Expected Launch : Oct 2025</t>
@@ -44,7 +44,7 @@
     <t>Honda Forza 350</t>
   </si>
   <si>
-    <t>Rs. 370000</t>
+    <t>370000</t>
   </si>
   <si>
     <t>Expected Launch : Unrevealed</t>
@@ -53,7 +53,7 @@
     <t>Honda CBR150R</t>
   </si>
   <si>
-    <t>Rs. 170000</t>
+    <t>170000</t>
   </si>
   <si>
     <t>Honda Rebel 300</t>
@@ -62,7 +62,7 @@
     <t>Honda PCX160</t>
   </si>
   <si>
-    <t>Rs. 120000</t>
+    <t>120000</t>
   </si>
   <si>
     <t>Honda Motocompacto</t>
@@ -74,7 +74,7 @@
     <t>Honda CRF300L</t>
   </si>
   <si>
-    <t>Rs. 330000</t>
+    <t>330000</t>
   </si>
 </sst>
 </file>

</xml_diff>